<commit_message>
i dunno what that is
</commit_message>
<xml_diff>
--- a/kvp-win32/bin/templates/calculation-sheet.xlsx
+++ b/kvp-win32/bin/templates/calculation-sheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>ЛС</t>
   </si>
@@ -22,33 +22,15 @@
     <t>№ комнат</t>
   </si>
   <si>
-    <t>Кол-во комнат</t>
-  </si>
-  <si>
     <t>Фамилия И.О.</t>
   </si>
   <si>
-    <t>Общая площадь</t>
-  </si>
-  <si>
-    <t>Техобслуживание</t>
-  </si>
-  <si>
     <t>Отопление</t>
   </si>
   <si>
     <t>Холодная вода</t>
   </si>
   <si>
-    <t>Канализация</t>
-  </si>
-  <si>
-    <t>Вывоз мусора</t>
-  </si>
-  <si>
-    <t>Электроэнергия</t>
-  </si>
-  <si>
     <t>Всего</t>
   </si>
   <si>
@@ -64,35 +46,59 @@
     <t>Услуги</t>
   </si>
   <si>
-    <t>Кол-во прожи-вающих</t>
-  </si>
-  <si>
     <t>Соц. найм</t>
   </si>
   <si>
-    <t>Техобслуживание:</t>
-  </si>
-  <si>
     <t>Отопление:</t>
   </si>
   <si>
-    <t>Холодное водоснабжение:</t>
-  </si>
-  <si>
     <t>Канализация:</t>
   </si>
   <si>
-    <t>Вывоз мусора:</t>
-  </si>
-  <si>
     <t>Электроэнергия:</t>
-  </si>
-  <si>
-    <t>Социальный наем:</t>
   </si>
   <si>
     <t>Ведомость расчетов с жильцами общежития
 ТОГБОУ СПО "Многоотраслевой техниум"</t>
+  </si>
+  <si>
+    <t>К-во ком.</t>
+  </si>
+  <si>
+    <t>Общ. пл.</t>
+  </si>
+  <si>
+    <t>К-во чел.</t>
+  </si>
+  <si>
+    <t>Ремонт и содерж.</t>
+  </si>
+  <si>
+    <t>Электро-энергия</t>
+  </si>
+  <si>
+    <t>Горячая вода</t>
+  </si>
+  <si>
+    <t>Газ</t>
+  </si>
+  <si>
+    <t>Канали-зация</t>
+  </si>
+  <si>
+    <t>Ремонт и содержание:</t>
+  </si>
+  <si>
+    <t>Холодная вода:</t>
+  </si>
+  <si>
+    <t>Горячая вода:</t>
+  </si>
+  <si>
+    <t>Газ:</t>
+  </si>
+  <si>
+    <t>Социальный найм:</t>
   </si>
 </sst>
 </file>
@@ -395,21 +401,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -436,50 +427,65 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -782,10 +788,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q12"/>
+  <dimension ref="A1:R13"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:Q1"/>
+      <selection activeCell="D5" sqref="D5:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -793,295 +799,334 @@
     <col min="1" max="1" width="4" style="1" customWidth="1"/>
     <col min="2" max="2" width="14.5703125" style="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="1" customWidth="1"/>
-    <col min="4" max="4" width="6.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="7.5703125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="7" style="1" customWidth="1"/>
+    <col min="4" max="6" width="4.7109375" style="1" customWidth="1"/>
     <col min="7" max="7" width="8.28515625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="8.85546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="1" customWidth="1"/>
     <col min="9" max="9" width="8" style="1" customWidth="1"/>
-    <col min="10" max="10" width="8.42578125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="7" style="1" customWidth="1"/>
-    <col min="12" max="12" width="7.5703125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="6.85546875" style="1" customWidth="1"/>
-    <col min="14" max="14" width="8.7109375" style="1" customWidth="1"/>
-    <col min="15" max="17" width="8.42578125" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.140625" style="1"/>
+    <col min="10" max="10" width="8.140625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="7.5703125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="7.28515625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="7.5703125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="7.28515625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="8.7109375" style="1" customWidth="1"/>
+    <col min="16" max="18" width="8.42578125" style="1" customWidth="1"/>
+    <col min="19" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
+      <c r="L1" s="40"/>
+      <c r="M1" s="40"/>
+      <c r="N1" s="40"/>
+      <c r="O1" s="40"/>
+      <c r="P1" s="40"/>
+      <c r="Q1" s="40"/>
+      <c r="R1" s="40"/>
+    </row>
+    <row r="2" spans="1:18" s="9" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="29"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="29"/>
+      <c r="P2" s="29"/>
+      <c r="Q2" s="29"/>
+      <c r="R2" s="29"/>
+    </row>
+    <row r="3" spans="1:18" s="9" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="29"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
+      <c r="K3" s="29"/>
+      <c r="L3" s="29"/>
+      <c r="M3" s="29"/>
+      <c r="N3" s="29"/>
+      <c r="O3" s="29"/>
+      <c r="P3" s="29"/>
+      <c r="Q3" s="29"/>
+      <c r="R3" s="29"/>
+    </row>
+    <row r="4" spans="1:18" s="9" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A4" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="36"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
-      <c r="O1" s="12"/>
-      <c r="P1" s="12"/>
-      <c r="Q1" s="12"/>
-    </row>
-    <row r="2" spans="1:17" s="9" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="15"/>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15"/>
-      <c r="L2" s="15"/>
-      <c r="M2" s="15"/>
-      <c r="N2" s="15"/>
-      <c r="O2" s="15"/>
-      <c r="P2" s="15"/>
-      <c r="Q2" s="15"/>
-    </row>
-    <row r="3" spans="1:17" s="9" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A3" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="G3" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
-    </row>
-    <row r="4" spans="1:17" s="9" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A4" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="G4" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14"/>
+      <c r="H4" s="36"/>
+      <c r="I4" s="36"/>
+      <c r="J4" s="28"/>
+      <c r="K4" s="28"/>
       <c r="L4" s="10"/>
       <c r="M4" s="10"/>
+      <c r="N4" s="10"/>
     </row>
-    <row r="5" spans="1:17" s="9" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="G5" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="14"/>
+    <row r="5" spans="1:18" s="9" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A5" s="36" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="36"/>
+      <c r="C5" s="36"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="36" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" s="36"/>
+      <c r="I5" s="36"/>
+      <c r="J5" s="28"/>
+      <c r="K5" s="28"/>
       <c r="L5" s="10"/>
       <c r="M5" s="10"/>
+      <c r="N5" s="10"/>
     </row>
-    <row r="6" spans="1:17" s="9" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A6" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
+    <row r="6" spans="1:18" s="9" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A6" s="36" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="36"/>
+      <c r="C6" s="36"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="36"/>
+      <c r="I6" s="36"/>
+      <c r="J6" s="28"/>
+      <c r="K6" s="28"/>
       <c r="L6" s="10"/>
       <c r="M6" s="10"/>
+      <c r="N6" s="10"/>
     </row>
-    <row r="7" spans="1:17" ht="12.75" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="26" t="s">
+    <row r="7" spans="1:18" s="9" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A7" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="36"/>
+      <c r="C7" s="36"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="H7" s="36"/>
+      <c r="I7" s="36"/>
+      <c r="J7" s="28"/>
+      <c r="K7" s="28"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
+      <c r="N7" s="10"/>
+    </row>
+    <row r="8" spans="1:18" ht="12.75" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="27" t="s">
+      <c r="B9" s="32" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="H9" s="32"/>
+      <c r="I9" s="32"/>
+      <c r="J9" s="32"/>
+      <c r="K9" s="32"/>
+      <c r="L9" s="32"/>
+      <c r="M9" s="32"/>
+      <c r="N9" s="32"/>
+      <c r="O9" s="32"/>
+      <c r="P9" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q9" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="R9" s="37" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="35"/>
+      <c r="B10" s="33"/>
+      <c r="C10" s="33"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="33"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="H10" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="D8" s="27" t="s">
-        <v>2</v>
-      </c>
-      <c r="E8" s="27" t="s">
+      <c r="I10" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="J10" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="F8" s="28" t="s">
-        <v>16</v>
-      </c>
-      <c r="G8" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="H8" s="27"/>
-      <c r="I8" s="27"/>
-      <c r="J8" s="27"/>
-      <c r="K8" s="27"/>
-      <c r="L8" s="27"/>
-      <c r="M8" s="27"/>
-      <c r="N8" s="27"/>
-      <c r="O8" s="27" t="s">
-        <v>12</v>
-      </c>
-      <c r="P8" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q8" s="29" t="s">
-        <v>14</v>
-      </c>
+      <c r="K10" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="L10" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="M10" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="N10" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="O10" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="P10" s="33"/>
+      <c r="Q10" s="33"/>
+      <c r="R10" s="38"/>
     </row>
-    <row r="9" spans="1:17" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="30"/>
-      <c r="B9" s="31"/>
-      <c r="C9" s="31"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="32"/>
-      <c r="G9" s="33" t="s">
-        <v>5</v>
-      </c>
-      <c r="H9" s="33" t="s">
-        <v>6</v>
-      </c>
-      <c r="I9" s="33" t="s">
-        <v>7</v>
-      </c>
-      <c r="J9" s="33" t="s">
-        <v>8</v>
-      </c>
-      <c r="K9" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="L9" s="33" t="s">
-        <v>10</v>
-      </c>
-      <c r="M9" s="33" t="s">
-        <v>17</v>
-      </c>
-      <c r="N9" s="33" t="s">
-        <v>11</v>
-      </c>
-      <c r="O9" s="31"/>
-      <c r="P9" s="31"/>
-      <c r="Q9" s="34"/>
+    <row r="11" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="17"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="22"/>
+      <c r="K11" s="22"/>
+      <c r="L11" s="22"/>
+      <c r="M11" s="22"/>
+      <c r="N11" s="22"/>
+      <c r="O11" s="22"/>
+      <c r="P11" s="22"/>
+      <c r="Q11" s="22"/>
+      <c r="R11" s="23"/>
     </row>
-    <row r="10" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="22"/>
-      <c r="B10" s="23"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="24"/>
-      <c r="G10" s="35"/>
-      <c r="H10" s="35"/>
-      <c r="I10" s="35"/>
-      <c r="J10" s="35"/>
-      <c r="K10" s="35"/>
-      <c r="L10" s="35"/>
-      <c r="M10" s="35"/>
-      <c r="N10" s="35"/>
-      <c r="O10" s="35"/>
-      <c r="P10" s="35"/>
-      <c r="Q10" s="36"/>
+    <row r="12" spans="1:18" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="7"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="24"/>
+      <c r="J12" s="24"/>
+      <c r="K12" s="24"/>
+      <c r="L12" s="24"/>
+      <c r="M12" s="24"/>
+      <c r="N12" s="24"/>
+      <c r="O12" s="24"/>
+      <c r="P12" s="24"/>
+      <c r="Q12" s="24"/>
+      <c r="R12" s="25"/>
     </row>
-    <row r="11" spans="1:17" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="37"/>
-      <c r="H11" s="37"/>
-      <c r="I11" s="37"/>
-      <c r="J11" s="37"/>
-      <c r="K11" s="37"/>
-      <c r="L11" s="37"/>
-      <c r="M11" s="37"/>
-      <c r="N11" s="37"/>
-      <c r="O11" s="37"/>
-      <c r="P11" s="37"/>
-      <c r="Q11" s="38"/>
-    </row>
-    <row r="12" spans="1:17" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="17"/>
-      <c r="B12" s="18"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="39"/>
-      <c r="H12" s="39"/>
-      <c r="I12" s="39"/>
-      <c r="J12" s="39"/>
-      <c r="K12" s="39"/>
-      <c r="L12" s="39"/>
-      <c r="M12" s="39"/>
-      <c r="N12" s="39"/>
-      <c r="O12" s="39"/>
-      <c r="P12" s="39"/>
-      <c r="Q12" s="40"/>
+    <row r="13" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="12"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="26"/>
+      <c r="H13" s="26"/>
+      <c r="I13" s="26"/>
+      <c r="J13" s="26"/>
+      <c r="K13" s="26"/>
+      <c r="L13" s="26"/>
+      <c r="M13" s="26"/>
+      <c r="N13" s="26"/>
+      <c r="O13" s="26"/>
+      <c r="P13" s="26"/>
+      <c r="Q13" s="26"/>
+      <c r="R13" s="27"/>
     </row>
   </sheetData>
-  <mergeCells count="28">
-    <mergeCell ref="G4:I4"/>
-    <mergeCell ref="G5:I5"/>
-    <mergeCell ref="A1:Q1"/>
+  <mergeCells count="29">
+    <mergeCell ref="A1:R1"/>
+    <mergeCell ref="A7:C7"/>
     <mergeCell ref="A6:C6"/>
     <mergeCell ref="A5:C5"/>
     <mergeCell ref="A4:C4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="A2:Q2"/>
-    <mergeCell ref="G6:I6"/>
-    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="A2:R2"/>
+    <mergeCell ref="G7:I7"/>
     <mergeCell ref="J4:K4"/>
     <mergeCell ref="J5:K5"/>
     <mergeCell ref="J6:K6"/>
-    <mergeCell ref="G3:I3"/>
-    <mergeCell ref="O8:O9"/>
-    <mergeCell ref="P8:P9"/>
-    <mergeCell ref="Q8:Q9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="G8:N8"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="P9:P10"/>
+    <mergeCell ref="Q9:Q10"/>
+    <mergeCell ref="R9:R10"/>
+    <mergeCell ref="G5:I5"/>
+    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="G9:O9"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="A3:R3"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="G4:I4"/>
   </mergeCells>
-  <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
+  <pageMargins left="0.35433070866141736" right="0.35433070866141736" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="landscape" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fixes, including a serious memory leak
</commit_message>
<xml_diff>
--- a/kvp-win32/bin/templates/calculation-sheet.xlsx
+++ b/kvp-win32/bin/templates/calculation-sheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="30">
   <si>
     <t>ЛС</t>
   </si>
@@ -25,12 +25,6 @@
     <t>Фамилия И.О.</t>
   </si>
   <si>
-    <t>Отопление</t>
-  </si>
-  <si>
-    <t>Холодная вода</t>
-  </si>
-  <si>
     <t>Всего</t>
   </si>
   <si>
@@ -46,59 +40,71 @@
     <t>Услуги</t>
   </si>
   <si>
-    <t>Соц. найм</t>
-  </si>
-  <si>
-    <t>Отопление:</t>
-  </si>
-  <si>
-    <t>Канализация:</t>
-  </si>
-  <si>
-    <t>Электроэнергия:</t>
+    <t>К-во ком.</t>
+  </si>
+  <si>
+    <t>Общ. пл.</t>
+  </si>
+  <si>
+    <t>К-во чел.</t>
+  </si>
+  <si>
+    <t>за {PERIOD_MONTH} {PERIOD_YEAR} года</t>
+  </si>
+  <si>
+    <t>{SERVICE_01_NAME}</t>
+  </si>
+  <si>
+    <t>{SERVICE_02_NAME}</t>
+  </si>
+  <si>
+    <t>{SERVICE_03_NAME}</t>
+  </si>
+  <si>
+    <t>{SERVICE_04_NAME}</t>
+  </si>
+  <si>
+    <t>{SERVICE_05_NAME}</t>
+  </si>
+  <si>
+    <t>{SERVICE_06_NAME}</t>
+  </si>
+  <si>
+    <t>{SERVICE_07_NAME}</t>
+  </si>
+  <si>
+    <t>{SERVICE_08_NAME}</t>
+  </si>
+  <si>
+    <t>{SERVICE_01_PRICE}</t>
+  </si>
+  <si>
+    <t>{SERVICE_03_PRICE}</t>
+  </si>
+  <si>
+    <t>{SERVICE_05_PRICE}</t>
+  </si>
+  <si>
+    <t>{SERVICE_07_PRICE}</t>
+  </si>
+  <si>
+    <t>{SERVICE_02_PRICE}</t>
+  </si>
+  <si>
+    <t>{SERVICE_04_PRICE}</t>
+  </si>
+  <si>
+    <t>{SERVICE_06_PRICE}</t>
+  </si>
+  <si>
+    <t>{SERVICE_08_PRICE}</t>
+  </si>
+  <si>
+    <t>{BUILDING_STREET}, {BUILDING_NUMBER}</t>
   </si>
   <si>
     <t>Ведомость расчетов с жильцами общежития
-ТОГБОУ СПО "Многоотраслевой техниум"</t>
-  </si>
-  <si>
-    <t>К-во ком.</t>
-  </si>
-  <si>
-    <t>Общ. пл.</t>
-  </si>
-  <si>
-    <t>К-во чел.</t>
-  </si>
-  <si>
-    <t>Ремонт и содерж.</t>
-  </si>
-  <si>
-    <t>Электро-энергия</t>
-  </si>
-  <si>
-    <t>Горячая вода</t>
-  </si>
-  <si>
-    <t>Газ</t>
-  </si>
-  <si>
-    <t>Канали-зация</t>
-  </si>
-  <si>
-    <t>Ремонт и содержание:</t>
-  </si>
-  <si>
-    <t>Холодная вода:</t>
-  </si>
-  <si>
-    <t>Горячая вода:</t>
-  </si>
-  <si>
-    <t>Газ:</t>
-  </si>
-  <si>
-    <t>Социальный найм:</t>
+{ORGANIZATION_SHORT_NAME}</t>
   </si>
 </sst>
 </file>
@@ -448,11 +454,32 @@
     <xf numFmtId="4" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -460,32 +487,11 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -791,7 +797,7 @@
   <dimension ref="A1:R13"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5:F5"/>
+      <selection activeCell="B9" sqref="B9:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -814,225 +820,245 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="39" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
-      <c r="I1" s="40"/>
-      <c r="J1" s="40"/>
-      <c r="K1" s="40"/>
-      <c r="L1" s="40"/>
-      <c r="M1" s="40"/>
-      <c r="N1" s="40"/>
-      <c r="O1" s="40"/>
-      <c r="P1" s="40"/>
-      <c r="Q1" s="40"/>
-      <c r="R1" s="40"/>
+      <c r="A1" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
+      <c r="O1" s="29"/>
+      <c r="P1" s="29"/>
+      <c r="Q1" s="29"/>
+      <c r="R1" s="29"/>
     </row>
     <row r="2" spans="1:18" s="9" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="29"/>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
-      <c r="K2" s="29"/>
-      <c r="L2" s="29"/>
-      <c r="M2" s="29"/>
-      <c r="N2" s="29"/>
-      <c r="O2" s="29"/>
-      <c r="P2" s="29"/>
-      <c r="Q2" s="29"/>
-      <c r="R2" s="29"/>
+      <c r="A2" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="31"/>
+      <c r="O2" s="31"/>
+      <c r="P2" s="31"/>
+      <c r="Q2" s="31"/>
+      <c r="R2" s="31"/>
     </row>
     <row r="3" spans="1:18" s="9" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="29"/>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
-      <c r="K3" s="29"/>
-      <c r="L3" s="29"/>
-      <c r="M3" s="29"/>
-      <c r="N3" s="29"/>
-      <c r="O3" s="29"/>
-      <c r="P3" s="29"/>
-      <c r="Q3" s="29"/>
-      <c r="R3" s="29"/>
+      <c r="A3" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="31"/>
+      <c r="L3" s="31"/>
+      <c r="M3" s="31"/>
+      <c r="N3" s="31"/>
+      <c r="O3" s="31"/>
+      <c r="P3" s="31"/>
+      <c r="Q3" s="31"/>
+      <c r="R3" s="31"/>
     </row>
     <row r="4" spans="1:18" s="9" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A4" s="36" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" s="36"/>
-      <c r="C4" s="36"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="36" t="s">
-        <v>25</v>
-      </c>
-      <c r="H4" s="36"/>
-      <c r="I4" s="36"/>
-      <c r="J4" s="28"/>
-      <c r="K4" s="28"/>
+      <c r="A4" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="30"/>
+      <c r="I4" s="30"/>
+      <c r="J4" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="K4" s="32"/>
       <c r="L4" s="10"/>
       <c r="M4" s="10"/>
       <c r="N4" s="10"/>
     </row>
     <row r="5" spans="1:18" s="9" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="36" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="36"/>
-      <c r="C5" s="36"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="28"/>
-      <c r="G5" s="36" t="s">
-        <v>26</v>
-      </c>
-      <c r="H5" s="36"/>
-      <c r="I5" s="36"/>
-      <c r="J5" s="28"/>
-      <c r="K5" s="28"/>
+      <c r="A5" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="30"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" s="30"/>
+      <c r="I5" s="30"/>
+      <c r="J5" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="K5" s="32"/>
       <c r="L5" s="10"/>
       <c r="M5" s="10"/>
       <c r="N5" s="10"/>
     </row>
     <row r="6" spans="1:18" s="9" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A6" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="36"/>
-      <c r="C6" s="36"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="28"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="36" t="s">
-        <v>12</v>
-      </c>
-      <c r="H6" s="36"/>
-      <c r="I6" s="36"/>
-      <c r="J6" s="28"/>
-      <c r="K6" s="28"/>
+      <c r="A6" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="30"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" s="30"/>
+      <c r="I6" s="30"/>
+      <c r="J6" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="K6" s="32"/>
       <c r="L6" s="10"/>
       <c r="M6" s="10"/>
       <c r="N6" s="10"/>
     </row>
     <row r="7" spans="1:18" s="9" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A7" s="36" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" s="36"/>
-      <c r="C7" s="36"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="28"/>
-      <c r="F7" s="28"/>
-      <c r="G7" s="36" t="s">
+      <c r="A7" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="30"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="32"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" s="30"/>
+      <c r="I7" s="30"/>
+      <c r="J7" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="H7" s="36"/>
-      <c r="I7" s="36"/>
-      <c r="J7" s="28"/>
-      <c r="K7" s="28"/>
+      <c r="K7" s="32"/>
       <c r="L7" s="10"/>
       <c r="M7" s="10"/>
       <c r="N7" s="10"/>
     </row>
     <row r="8" spans="1:18" ht="12.75" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="34" t="s">
+      <c r="A9" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="32" t="s">
+      <c r="B9" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="32" t="s">
+      <c r="C9" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="32" t="s">
+      <c r="D9" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="H9" s="33"/>
+      <c r="I9" s="33"/>
+      <c r="J9" s="33"/>
+      <c r="K9" s="33"/>
+      <c r="L9" s="33"/>
+      <c r="M9" s="33"/>
+      <c r="N9" s="33"/>
+      <c r="O9" s="33"/>
+      <c r="P9" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q9" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="R9" s="35" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" s="2" customFormat="1" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="40"/>
+      <c r="B10" s="34"/>
+      <c r="C10" s="34"/>
+      <c r="D10" s="34"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="H10" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="I10" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="J10" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="32" t="s">
+      <c r="K10" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="30" t="s">
+      <c r="L10" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="G9" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="H9" s="32"/>
-      <c r="I9" s="32"/>
-      <c r="J9" s="32"/>
-      <c r="K9" s="32"/>
-      <c r="L9" s="32"/>
-      <c r="M9" s="32"/>
-      <c r="N9" s="32"/>
-      <c r="O9" s="32"/>
-      <c r="P9" s="32" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q9" s="32" t="s">
-        <v>7</v>
-      </c>
-      <c r="R9" s="37" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="35"/>
-      <c r="B10" s="33"/>
-      <c r="C10" s="33"/>
-      <c r="D10" s="33"/>
-      <c r="E10" s="33"/>
-      <c r="F10" s="31"/>
-      <c r="G10" s="21" t="s">
+      <c r="M10" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="H10" s="21" t="s">
+      <c r="N10" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="O10" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="I10" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="J10" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="K10" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="L10" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="M10" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="N10" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="O10" s="21" t="s">
-        <v>5</v>
-      </c>
-      <c r="P10" s="33"/>
-      <c r="Q10" s="33"/>
-      <c r="R10" s="38"/>
+      <c r="P10" s="34"/>
+      <c r="Q10" s="34"/>
+      <c r="R10" s="36"/>
     </row>
     <row r="11" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="17"/>
@@ -1096,6 +1122,19 @@
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="G9:O9"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="P9:P10"/>
+    <mergeCell ref="Q9:Q10"/>
+    <mergeCell ref="R9:R10"/>
+    <mergeCell ref="G5:I5"/>
+    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="J7:K7"/>
     <mergeCell ref="A1:R1"/>
     <mergeCell ref="A7:C7"/>
     <mergeCell ref="A6:C6"/>
@@ -1106,27 +1145,14 @@
     <mergeCell ref="J4:K4"/>
     <mergeCell ref="J5:K5"/>
     <mergeCell ref="J6:K6"/>
-    <mergeCell ref="P9:P10"/>
-    <mergeCell ref="Q9:Q10"/>
-    <mergeCell ref="R9:R10"/>
-    <mergeCell ref="G5:I5"/>
-    <mergeCell ref="G6:I6"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="G9:O9"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
     <mergeCell ref="D4:F4"/>
     <mergeCell ref="D5:F5"/>
     <mergeCell ref="D6:F6"/>
     <mergeCell ref="D7:F7"/>
     <mergeCell ref="A3:R3"/>
-    <mergeCell ref="J7:K7"/>
     <mergeCell ref="G4:I4"/>
   </mergeCells>
   <pageMargins left="0.35433070866141736" right="0.35433070866141736" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
-  <pageSetup paperSize="9" orientation="landscape" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>